<commit_message>
Created training and test split and added loading of data with bare-minimum Classifier
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="78">
   <si>
     <t>classification</t>
   </si>
@@ -154,21 +154,6 @@
     <t>8.8.8.8:53 224.0.0.252:5355 192.168.56.255:137 239.255.255.250:3702 239.255.255.250:1900 239.255.255.250:1900 224.0.0.252:5355 239.255.255.250:3702 8.8.8.8:53 192.168.56.255:138 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 239.255.255.250:3702 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355</t>
   </si>
   <si>
-    <t>SINGLETON:01e294060904e9a60742f95dd1079594</t>
-  </si>
-  <si>
-    <t>01e294060904e9a60742f95dd1079594</t>
-  </si>
-  <si>
-    <t>LdrGetDllHandle LdrGetDllHandle IsDebuggerPresent NtQuerySystemInformation NtQuerySystemInformation NtAllocateVirtualMemory NtQuerySystemInformation NtCreateFile GetFileSize NtCreateSection NtMapViewOfSection NtUnmapViewOfSection NtClose NtClose NtProtectVirtualMemory NtProtectVirtualMemory NtProtectVirtualMemory NtProtectVirtualMemory NtProtectVirtualMemory LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle LdrGetDllHandle NtClose __exception__ OpenSCManagerW NtCreateThreadEx NtDuplicateObject NtResumeThread LdrLoadDll MessageBoxTimeoutW LdrUnloadDll NtTerminateProcess NtTerminateProcess NtClose NtClose NtClose NtClose LdrUnloadDll NtOpenKey NtQueryValueKey NtClose NtClose NtClose NtClose NtClose NtTerminateProcess</t>
-  </si>
-  <si>
-    <t>192.168.56.101:49360 192.168.56.101:64412 192.168.56.101:50300 192.168.56.101:137 192.168.56.101:1900 192.168.56.101:64414 192.168.56.101:64416 192.168.56.101:138 192.168.56.101:58084 192.168.56.101:54425 192.168.56.101:54426 192.168.56.101:52057 192.168.56.101:59469 192.168.56.101:54227 192.168.56.101:54228 192.168.56.101:52887 192.168.56.101:63529 192.168.56.101:51765</t>
-  </si>
-  <si>
-    <t>224.0.0.252:5355 8.8.8.8:53 239.255.255.250:3702 192.168.56.255:137 239.255.255.250:1900 239.255.255.250:1900 239.255.255.250:3702 192.168.56.255:138 224.0.0.252:5355 8.8.8.8:53 239.255.255.250:3702 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 239.255.255.250:3702 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355</t>
-  </si>
-  <si>
     <t>022c025365bc4875a116877a3d2648a6</t>
   </si>
   <si>
@@ -236,48 +221,6 @@
   </si>
   <si>
     <t>8.8.8.8:53 239.255.255.250:3702 224.0.0.252:5355 192.168.56.255:137 239.255.255.250:1900 239.255.255.250:1900 239.255.255.250:3702 192.168.56.255:138 239.255.255.250:3702 224.0.0.252:5355 8.8.8.8:53 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 239.255.255.250:3702 239.255.255.250:3702 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 224.0.0.252:5355 8.8.8.8:53 8.8.8.8:53 224.0.0.252:5355 8.8.8.8:53</t>
-  </si>
-  <si>
-    <t>SINGLETON:02e3ab3984b3c0875fbf369145c1c3df</t>
-  </si>
-  <si>
-    <t>02e3ab3984b3c0875fbf369145c1c3df</t>
-  </si>
-  <si>
-    <t>GetSystemTimeAsFileTime SetUnhandledExceptionFilter SetErrorMode GetFileAttributesW GetFileAttributesW CreateActCtxW CreateActCtxW CreateActCtxW NtClose LdrLoadDll NtCreateFile NtReadFile SetFilePointer NtReadFile NtClose CreateProcessInternalW NtClose NtClose NtTerminateProcess NtTerminateProcess NtClose LdrUnloadDll NtOpenKey NtQueryValueKey NtClose NtTerminateProcess</t>
-  </si>
-  <si>
-    <t>192.168.56.101:49360 192.168.56.101:64412 192.168.56.101:58084 192.168.56.101:54425 192.168.56.101:52057 192.168.56.101:59469 192.168.56.101:54227 192.168.56.101:52887 192.168.56.101:50300 192.168.56.101:137 192.168.56.101:1900 192.168.56.101:52889 192.168.56.101:63529 192.168.56.101:51765 192.168.56.101:51766 192.168.56.101:49465 192.168.56.101:138</t>
-  </si>
-  <si>
-    <t>224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 239.255.255.250:3702 192.168.56.255:137 239.255.255.250:1900 239.255.255.250:1900 224.0.0.252:5355 224.0.0.252:5355 239.255.255.250:3702 8.8.8.8:53 192.168.56.255:138</t>
-  </si>
-  <si>
-    <t>SINGLETON:0306f7cc5a0b6f4a52c17c14121d5c48</t>
-  </si>
-  <si>
-    <t>0306f7cc5a0b6f4a52c17c14121d5c48</t>
-  </si>
-  <si>
-    <t>192.168.56.101:49360 192.168.56.101:64412 192.168.56.101:58084 192.168.56.101:54425 192.168.56.101:52057 192.168.56.101:59469 192.168.56.101:54227 192.168.56.101:50300 192.168.56.101:137 192.168.56.101:1900 192.168.56.101:54229 192.168.56.101:52887 192.168.56.101:63529 192.168.56.101:63530 192.168.56.101:51765 192.168.56.101:51766 192.168.56.101:49465 192.168.56.101:138</t>
-  </si>
-  <si>
-    <t>224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 239.255.255.250:3702 192.168.56.255:137 239.255.255.250:1900 239.255.255.250:1900 224.0.0.252:5355 224.0.0.252:5355 239.255.255.250:3702 224.0.0.252:5355 239.255.255.250:3702 8.8.8.8:53 192.168.56.255:138</t>
-  </si>
-  <si>
-    <t>SINGLETON:039114efafc6e003500920d0bec22dfa</t>
-  </si>
-  <si>
-    <t>039114efafc6e003500920d0bec22dfa</t>
-  </si>
-  <si>
-    <t>LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrLoadDll LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress LdrGetProcedureAddress NtProtectVirtualMemory NtProtectVirtualMemory NtAllocateVirtualMemory NtFreeVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtAllocateVirtualMemory NtFreeVirtualMemory NtAllocateVirtualMemory FindResourceExW LoadResource FindResourceExW LoadResource NtAllocateVirtualMemory NtAllocateVirtualMemory NtFreeVirtualMemory NtAllocateVirtualMemory CoInitializeEx NtAllocateVirtualMemory NtClose NtOpenKey NtQueryValueKey NtClose NtOpenKey NtQueryValueKey NtClose FindResourceExW LoadResource SetUnhandledExceptionFilter FindResourceA LoadResource SizeofResource NtAllocateVirtualMemory GetTempPathW LdrLoadDll LdrGetProcedureAddress SetErrorMode GetFileAttributesW FindFirstFileExW NtClose FindFirstFileExW NtClose FindFirstFileExW NtClose FindFirstFileExW NtClose FindFirstFileExW NtClose SetErrorMode LdrUnloadDll GetFileAttributesW NtCreateFile NtClose DeleteFileW CreateDirectoryW FindResourceA LoadResource SizeofResource FindResourceA LoadResource SizeofResource FindResourceA LoadResource SizeofResource FindResourceA LoadResource SizeofResource FindResourceA NtAllocateVirtualMemory FindResourceA NtCreateFile SetFilePointer NtWriteFile NtWriteFile NtWriteFile NtClose NtOpenFile NtClose NtCreateFile NtCreateFile SetFilePointer NtWriteFile NtWriteFile NtWriteFile NtClose NtCreateFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtReadFile NtClose NtOpenFile NtOpenFile NtDuplicateObject NtClose CreateProcessInternalW NtClose NtClose</t>
-  </si>
-  <si>
-    <t>192.168.56.101:49360 192.168.56.101:64412 192.168.56.101:58084 192.168.56.101:54425 192.168.56.101:52057 192.168.56.101:50300 192.168.56.101:137 192.168.56.101:1900 192.168.56.101:52059 192.168.56.101:59469 192.168.56.101:54227 192.168.56.101:54228 192.168.56.101:52887 192.168.56.101:52888 192.168.56.101:63529 192.168.56.101:138 192.168.56.101:51765</t>
-  </si>
-  <si>
-    <t>224.0.0.252:5355 224.0.0.252:5355 224.0.0.252:5355 8.8.8.8:53 224.0.0.252:5355 239.255.255.250:3702 192.168.56.255:137 239.255.255.250:1900 239.255.255.250:1900 224.0.0.252:5355 224.0.0.252:5355 239.255.255.250:3702 224.0.0.252:5355 239.255.255.250:3702 8.8.8.8:53 192.168.56.255:138 224.0.0.252:5355</t>
   </si>
   <si>
     <t>03ad0aea1dc1f1fd3d9c441a063f23e6</t>
@@ -636,7 +579,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -811,19 +754,19 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
         <v>46</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>47</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>48</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>49</v>
-      </c>
-      <c r="E11" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -831,21 +774,21 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
         <v>51</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>52</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>53</v>
-      </c>
-      <c r="E12" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
         <v>55</v>
@@ -896,101 +839,36 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
         <v>69</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>70</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>71</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>72</v>
-      </c>
-      <c r="E16" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
         <v>74</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>75</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>76</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>77</v>
-      </c>
-      <c r="E17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>83</v>
-      </c>
-      <c r="B19" t="s">
-        <v>84</v>
-      </c>
-      <c r="C19" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D20" t="s">
-        <v>90</v>
-      </c>
-      <c r="E20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>92</v>
-      </c>
-      <c r="B21" t="s">
-        <v>93</v>
-      </c>
-      <c r="C21" t="s">
-        <v>94</v>
-      </c>
-      <c r="D21" t="s">
-        <v>95</v>
-      </c>
-      <c r="E21" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>